<commit_message>
add etl tables for vitals, labs/imaging
</commit_message>
<xml_diff>
--- a/ETL_Concepts.xlsx
+++ b/ETL_Concepts.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="3040" windowWidth="19200" windowHeight="7520" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="3420" windowWidth="19200" windowHeight="7520" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="7" r:id="rId1"/>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="744" uniqueCount="464">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="766" uniqueCount="476">
   <si>
     <t>concept_id</t>
   </si>
@@ -1424,6 +1424,42 @@
   </si>
   <si>
     <t>hiv_vl_quant</t>
+  </si>
+  <si>
+    <t>a8a65fee-1350-11df-a1f1-0026b9348838</t>
+  </si>
+  <si>
+    <t>TEMPERATURE (C)</t>
+  </si>
+  <si>
+    <t>a8a66354-1350-11df-a1f1-0026b9348838</t>
+  </si>
+  <si>
+    <t>BLOOD OXYGEN SATURATION</t>
+  </si>
+  <si>
+    <t>SYSTOLIC BLOOD PRESSURE</t>
+  </si>
+  <si>
+    <t>a8a65d5a-1350-11df-a1f1-0026b9348838</t>
+  </si>
+  <si>
+    <t>a8a65e36-1350-11df-a1f1-0026b9348838</t>
+  </si>
+  <si>
+    <t>DIASTOLIC BLOOD PRESSURE</t>
+  </si>
+  <si>
+    <t>PULSE</t>
+  </si>
+  <si>
+    <t>a8a65f12-1350-11df-a1f1-0026b9348838</t>
+  </si>
+  <si>
+    <t>AST</t>
+  </si>
+  <si>
+    <t>X-RAY, CHEST, PRELIMINARY FINDINGS</t>
   </si>
 </sst>
 </file>
@@ -3463,10 +3499,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J146"/>
+  <dimension ref="A1:J156"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A39" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="C47" sqref="C47"/>
+    <sheetView tabSelected="1" topLeftCell="A54" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="C63" sqref="C63"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -7840,10 +7876,127 @@
       <c r="G145" s="3"/>
     </row>
     <row r="146" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="B146" s="2"/>
-      <c r="C146" s="2"/>
+      <c r="A146" s="3">
+        <v>5089</v>
+      </c>
+      <c r="B146" s="1" t="s">
+        <v>348</v>
+      </c>
+      <c r="C146" s="1" t="s">
+        <v>347</v>
+      </c>
       <c r="D146" s="2"/>
       <c r="E146" s="2"/>
+    </row>
+    <row r="147" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A147" s="3">
+        <v>5090</v>
+      </c>
+      <c r="B147" s="1" t="s">
+        <v>350</v>
+      </c>
+      <c r="C147" s="1" t="s">
+        <v>351</v>
+      </c>
+    </row>
+    <row r="148" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A148" s="3">
+        <v>5088</v>
+      </c>
+      <c r="B148" s="1" t="s">
+        <v>464</v>
+      </c>
+      <c r="C148" s="1" t="s">
+        <v>465</v>
+      </c>
+    </row>
+    <row r="149" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A149" s="3">
+        <v>5092</v>
+      </c>
+      <c r="B149" s="1" t="s">
+        <v>466</v>
+      </c>
+      <c r="C149" s="1" t="s">
+        <v>467</v>
+      </c>
+    </row>
+    <row r="150" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A150" s="3">
+        <v>5085</v>
+      </c>
+      <c r="B150" s="1" t="s">
+        <v>469</v>
+      </c>
+      <c r="C150" s="1" t="s">
+        <v>468</v>
+      </c>
+    </row>
+    <row r="151" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A151" s="3">
+        <v>5086</v>
+      </c>
+      <c r="B151" s="1" t="s">
+        <v>470</v>
+      </c>
+      <c r="C151" s="1" t="s">
+        <v>471</v>
+      </c>
+    </row>
+    <row r="152" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A152" s="3">
+        <v>5087</v>
+      </c>
+      <c r="B152" s="1" t="s">
+        <v>473</v>
+      </c>
+      <c r="C152" s="1" t="s">
+        <v>472</v>
+      </c>
+    </row>
+    <row r="153" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A153" s="3">
+        <v>21</v>
+      </c>
+      <c r="B153" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C153" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="154" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A154" s="3">
+        <v>653</v>
+      </c>
+      <c r="B154" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="C154" s="1" t="s">
+        <v>474</v>
+      </c>
+    </row>
+    <row r="155" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A155" s="3">
+        <v>790</v>
+      </c>
+      <c r="B155" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="C155" s="1" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="156" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A156" s="3">
+        <v>12</v>
+      </c>
+      <c r="B156" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C156" s="1" t="s">
+        <v>475</v>
+      </c>
     </row>
   </sheetData>
   <autoFilter ref="A1:H145">

</xml_diff>